<commit_message>
done sản phẩm trong bảng thông số ver1
</commit_message>
<xml_diff>
--- a/Document/ThongSoSanPham.xlsx
+++ b/Document/ThongSoSanPham.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\So Hoang Tung 2017\HH\file exel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectShop_NK\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADDE782-F2E4-44FE-B2DE-71AC2698AF54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -244,7 +243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -266,7 +265,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +275,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -345,11 +356,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1456,18 +1470,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1490,10 +1504,10 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="4"/>
@@ -1502,7 +1516,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1514,7 +1528,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1526,7 +1540,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1538,10 +1552,10 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="4"/>
@@ -1550,7 +1564,7 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -1559,10 +1573,10 @@
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1574,7 +1588,7 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1586,19 +1600,19 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1610,7 +1624,7 @@
       <c r="A12" s="5">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -1622,7 +1636,7 @@
       <c r="A13" s="5">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1634,7 +1648,7 @@
       <c r="A14" s="5">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -1646,7 +1660,7 @@
       <c r="A15" s="5">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -1658,7 +1672,7 @@
       <c r="A16" s="5">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -1670,7 +1684,7 @@
       <c r="A17" s="5">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="11" t="s">

</xml_diff>